<commit_message>
Text edits, README.md update and bug fixes
</commit_message>
<xml_diff>
--- a/dashboard/Data/Electricity_demand.xlsx
+++ b/dashboard/Data/Electricity_demand.xlsx
@@ -84,21 +84,12 @@
     <t>Cooling</t>
   </si>
   <si>
-    <t>Electrical appliances</t>
-  </si>
-  <si>
     <t>Cooling new users</t>
   </si>
   <si>
-    <t>Electrical appliances new users</t>
-  </si>
-  <si>
     <t>Commercial electricity</t>
   </si>
   <si>
-    <t>Electricity appliances</t>
-  </si>
-  <si>
     <t>Other uses</t>
   </si>
   <si>
@@ -111,9 +102,6 @@
     <t>TRA_BUS_ELC_001</t>
   </si>
   <si>
-    <t>Car</t>
-  </si>
-  <si>
     <t>TRA_CAR_ELC_001</t>
   </si>
   <si>
@@ -136,6 +124,18 @@
   </si>
   <si>
     <t>Fuel</t>
+  </si>
+  <si>
+    <t>Residential appliances</t>
+  </si>
+  <si>
+    <t>Residential appliances new users</t>
+  </si>
+  <si>
+    <t>Cars</t>
+  </si>
+  <si>
+    <t>Commercial uses</t>
   </si>
 </sst>
 </file>
@@ -496,7 +496,7 @@
   <dimension ref="A1:J13"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="D12" sqref="D12"/>
+      <selection activeCell="D10" sqref="D10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -504,7 +504,7 @@
     <col min="1" max="1" width="21" customWidth="1"/>
     <col min="2" max="2" width="25.36328125" customWidth="1"/>
     <col min="3" max="3" width="20.81640625" customWidth="1"/>
-    <col min="4" max="4" width="27.1796875" customWidth="1"/>
+    <col min="4" max="4" width="28.6328125" bestFit="1" customWidth="1"/>
     <col min="5" max="27" width="20.81640625" customWidth="1"/>
   </cols>
   <sheetData>
@@ -522,7 +522,7 @@
         <v>15</v>
       </c>
       <c r="E1" s="4" t="s">
-        <v>38</v>
+        <v>34</v>
       </c>
       <c r="F1" s="5"/>
       <c r="I1" s="5"/>
@@ -556,7 +556,7 @@
         <v>9</v>
       </c>
       <c r="D3" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="E3" t="s">
         <v>14</v>
@@ -590,7 +590,7 @@
         <v>9</v>
       </c>
       <c r="D5" t="s">
-        <v>21</v>
+        <v>35</v>
       </c>
       <c r="E5" t="s">
         <v>14</v>
@@ -607,7 +607,7 @@
         <v>9</v>
       </c>
       <c r="D6" t="s">
-        <v>23</v>
+        <v>36</v>
       </c>
       <c r="E6" t="s">
         <v>14</v>
@@ -615,7 +615,7 @@
     </row>
     <row r="7" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A7" s="2" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
       <c r="B7" s="1" t="s">
         <v>0</v>
@@ -624,7 +624,7 @@
         <v>10</v>
       </c>
       <c r="D7" t="s">
-        <v>25</v>
+        <v>38</v>
       </c>
       <c r="E7" t="s">
         <v>14</v>
@@ -632,16 +632,16 @@
     </row>
     <row r="8" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A8" s="2" t="s">
-        <v>27</v>
+        <v>24</v>
       </c>
       <c r="B8" s="1" t="s">
-        <v>29</v>
+        <v>26</v>
       </c>
       <c r="C8" t="s">
         <v>11</v>
       </c>
       <c r="D8" t="s">
-        <v>28</v>
+        <v>25</v>
       </c>
       <c r="E8" t="s">
         <v>14</v>
@@ -649,16 +649,16 @@
     </row>
     <row r="9" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A9" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="B9" s="1" t="s">
         <v>27</v>
-      </c>
-      <c r="B9" s="1" t="s">
-        <v>31</v>
       </c>
       <c r="C9" t="s">
         <v>11</v>
       </c>
       <c r="D9" t="s">
-        <v>30</v>
+        <v>37</v>
       </c>
       <c r="E9" t="s">
         <v>14</v>
@@ -666,16 +666,16 @@
     </row>
     <row r="10" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A10" s="2" t="s">
-        <v>27</v>
+        <v>24</v>
       </c>
       <c r="B10" s="1" t="s">
-        <v>32</v>
+        <v>28</v>
       </c>
       <c r="C10" t="s">
         <v>11</v>
       </c>
       <c r="D10" t="s">
-        <v>34</v>
+        <v>30</v>
       </c>
       <c r="E10" t="s">
         <v>14</v>
@@ -683,16 +683,16 @@
     </row>
     <row r="11" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A11" s="2" t="s">
-        <v>27</v>
+        <v>24</v>
       </c>
       <c r="B11" s="1" t="s">
-        <v>33</v>
+        <v>29</v>
       </c>
       <c r="C11" t="s">
         <v>11</v>
       </c>
       <c r="D11" t="s">
-        <v>34</v>
+        <v>30</v>
       </c>
       <c r="E11" t="s">
         <v>14</v>
@@ -700,7 +700,7 @@
     </row>
     <row r="12" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A12" s="2" t="s">
-        <v>35</v>
+        <v>31</v>
       </c>
       <c r="B12" s="1" t="s">
         <v>1</v>
@@ -709,7 +709,7 @@
         <v>12</v>
       </c>
       <c r="D12" t="s">
-        <v>36</v>
+        <v>32</v>
       </c>
       <c r="E12" t="s">
         <v>14</v>
@@ -717,7 +717,7 @@
     </row>
     <row r="13" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A13" s="2" t="s">
-        <v>37</v>
+        <v>33</v>
       </c>
       <c r="B13" s="1" t="s">
         <v>2</v>
@@ -726,7 +726,7 @@
         <v>13</v>
       </c>
       <c r="D13" t="s">
-        <v>26</v>
+        <v>23</v>
       </c>
       <c r="E13" t="s">
         <v>14</v>

</xml_diff>